<commit_message>
Fixed Id override on bar update. Symetric xls_update / export implemented.
</commit_message>
<xml_diff>
--- a/dramatis_personae_update.xlsx
+++ b/dramatis_personae_update.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4276" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4710" uniqueCount="956">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -2589,51 +2589,288 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Addiction</t>
   </si>
   <si>
     <t xml:space="preserve">ba</t>
   </si>
   <si>
+    <t xml:space="preserve">FS2CRB</t>
+  </si>
+  <si>
     <t xml:space="preserve">-3</t>
   </si>
   <si>
     <t xml:space="preserve">-4</t>
   </si>
   <si>
+    <t xml:space="preserve">Adept Robes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alien Upbringing</t>
   </si>
   <si>
+    <t xml:space="preserve">Ally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article of Faith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black sheep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1500</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cloistered</t>
   </si>
   <si>
+    <t xml:space="preserve">Cohort Badge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dean / Master / Dean / Colonel / Dean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Captain / Crafter / Jonin / Captain / Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consul  / Engineer / Consul / Major / Consul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commander / Fellow / Boss / Lieutenant / Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enseign / Apprentice / Associate / Private / Associate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieutenant / Entered / Genin / Sergeant / Chief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dark Secret</t>
   </si>
   <si>
+    <t xml:space="preserve">Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escaped Serf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escaped Slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excommunicated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallen from Grace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Ties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gossip Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Known Worlds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An entire Royale House’s holdings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planetwide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City or Community</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heir</t>
   </si>
   <si>
+    <t xml:space="preserve">Householder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imperial Charter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indebted</t>
+  </si>
+  <si>
     <t xml:space="preserve">Infamous Family</t>
   </si>
   <si>
+    <t xml:space="preserve">Jumpkey</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lost Worlder</t>
   </si>
   <si>
+    <t xml:space="preserve">Mist sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural Disrupter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight (Minor house)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oath of Fealty</t>
   </si>
   <si>
     <t xml:space="preserve">Obligation</t>
   </si>
   <si>
+    <t xml:space="preserve">Ordained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archbishop / Grand Master / Presbuteros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bishop / Master / Magister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priest / Adept / Philosophus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deacon / Acolyte / Illuminatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canon / Oblate / Provost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novitiate / Apprentice / Novitiate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orphan</t>
   </si>
   <si>
+    <t xml:space="preserve">Outlaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passage Contract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ship at your command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luxury Liner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stateroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tramp Freighter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional Contract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psi Cloak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Military Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monastery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guild Safe House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retinue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint’s Lore</t>
+  </si>
+  <si>
     <t xml:space="preserve">Secrets</t>
   </si>
   <si>
     <t xml:space="preserve">Stigma</t>
   </si>
   <si>
+    <t xml:space="preserve">Vendetta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vestments</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vow of Celibacy</t>
   </si>
   <si>
@@ -2646,190 +2883,24 @@
     <t xml:space="preserve">Well-Traveled</t>
   </si>
   <si>
+    <t xml:space="preserve">Known Worlds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Major house Fief</t>
   </si>
   <si>
-    <t xml:space="preserve">Known Worlds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family Ties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gossip Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City or Community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planetwide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An entire Royale House’s holdings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Known Worlds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendetta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumpkey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">po</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passage Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tramp Freighter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stateroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luxury Liner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ship at your command</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small Farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guild Safe House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monastery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Military Base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux sword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mist sword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neural Disrupter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psi Cloak</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wireblade</t>
   </si>
   <si>
-    <t xml:space="preserve">Adept Robes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Article of Faith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saint’s Lore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vestments</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wyrd Tabernacle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indebted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cohort Badge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">st</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Enseign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Lieutenant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Commander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Captain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Consul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Dean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Apprentice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Entered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Fellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Crafter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Associate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Genin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Boss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commission – Jonin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -2919,7 +2990,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2932,8 +3003,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3022,7 +3097,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.76"/>
   </cols>
   <sheetData>
@@ -3075,12 +3150,12 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="9" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="8.76"/>
   </cols>
@@ -12279,7 +12354,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.76"/>
@@ -14932,12 +15007,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.76"/>
   </cols>
   <sheetData>
@@ -15668,27 +15743,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="8.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.76"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>524</v>
       </c>
@@ -15701,1718 +15778,3143 @@
       <c r="D2" s="2" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>539</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>854</v>
-      </c>
       <c r="B4" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>856</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>854</v>
-      </c>
       <c r="B5" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>591</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>859</v>
+        <v>101</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>580</v>
+        <v>44</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>580</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>856</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>539</v>
+        <v>864</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>856</v>
+        <v>429</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>53</v>
+        <v>428</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>580</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>863</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>580</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>670</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>864</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>864</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>865</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>865</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>865</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>866</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>867</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="B27" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>868</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>856</v>
+        <v>428</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>857</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>580</v>
+        <v>43</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>539</v>
+        <v>45</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>856</v>
+        <v>44</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>872</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>855</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>855</v>
+        <v>861</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>597</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>875</v>
+        <v>866</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>553</v>
+        <v>41</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>2</v>
+        <v>866</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>3</v>
+        <v>873</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>4</v>
+      <c r="B38" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>5</v>
+      <c r="B39" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>6</v>
+      <c r="B40" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>7</v>
+        <v>876</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>8</v>
+        <v>877</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>864</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>9</v>
+        <v>877</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>10</v>
+        <v>877</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>428</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>11</v>
+        <v>877</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>876</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>1</v>
+        <v>877</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>877</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>3</v>
+      <c r="B47" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>1</v>
+        <v>877</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>879</v>
+        <v>592</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>2</v>
+        <v>877</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>880</v>
+        <v>841</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>3</v>
+        <v>877</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>881</v>
+        <v>836</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>4</v>
+        <v>877</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>882</v>
+        <v>849</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>883</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>3</v>
+        <v>877</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>670</v>
+        <v>861</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>884</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
+        <v>881</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>670</v>
+        <v>856</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>884</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>2</v>
+        <v>882</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>883</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>884</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>670</v>
+      <c r="E55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>884</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>4</v>
+        <v>883</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>428</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>885</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>-1</v>
+        <v>883</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>886</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>886</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>-1</v>
+        <v>883</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>886</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <v>-2</v>
+        <v>883</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>888</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>886</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>-3</v>
+        <v>883</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>670</v>
+        <v>874</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>889</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>886</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>-4</v>
+        <v>890</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>887</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>2</v>
+        <v>891</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>888</v>
+        <v>856</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>889</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>2</v>
+        <v>891</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>890</v>
+        <v>856</v>
+      </c>
+      <c r="E63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>889</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>4</v>
+        <v>891</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>891</v>
+        <v>856</v>
+      </c>
+      <c r="E64" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>889</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <v>6</v>
+        <v>892</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>892</v>
+        <v>670</v>
+      </c>
+      <c r="E65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>889</v>
-      </c>
-      <c r="B66" s="0" t="n">
-        <v>8</v>
+        <v>893</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>893</v>
+        <v>874</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>889</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>10</v>
+        <v>894</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>894</v>
+        <v>874</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>895</v>
       </c>
-      <c r="B68" s="0" t="n">
-        <v>2</v>
+      <c r="B68" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>896</v>
+        <v>874</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>895</v>
-      </c>
-      <c r="B69" s="0" t="n">
-        <v>4</v>
+        <v>896</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>897</v>
+        <v>874</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>895</v>
-      </c>
-      <c r="B70" s="0" t="n">
-        <v>6</v>
+        <v>896</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>898</v>
+        <v>874</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>895</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>8</v>
+        <v>896</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>899</v>
+        <v>874</v>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>895</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>10</v>
+        <v>897</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>900</v>
+        <v>670</v>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <v>5</v>
+        <v>898</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>864</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>901</v>
-      </c>
-      <c r="B74" s="0" t="n">
-        <v>11</v>
+        <v>899</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>888</v>
+        <v>670</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>902</v>
-      </c>
-      <c r="B75" s="0" t="n">
-        <v>13</v>
+        <v>899</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>888</v>
+        <v>670</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>903</v>
-      </c>
-      <c r="B76" s="0" t="n">
-        <v>10</v>
+        <v>899</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>888</v>
+        <v>670</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>902</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>904</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>10</v>
+        <v>899</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>888</v>
+        <v>670</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>905</v>
-      </c>
-      <c r="B78" s="0" t="n">
-        <v>12</v>
+        <v>904</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>888</v>
+        <v>856</v>
+      </c>
+      <c r="E78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>906</v>
-      </c>
-      <c r="B79" s="0" t="n">
-        <v>20</v>
+        <v>905</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>907</v>
-      </c>
-      <c r="B80" s="0" t="n">
-        <v>1</v>
+        <v>906</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="B81" s="0" t="n">
-        <v>2</v>
+      <c r="B81" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="B82" s="0" t="n">
-        <v>3</v>
+      <c r="B82" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="B83" s="0" t="n">
-        <v>4</v>
+      <c r="B83" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="B84" s="0" t="n">
-        <v>5</v>
+      <c r="B84" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="B85" s="0" t="n">
-        <v>6</v>
+      <c r="B85" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>908</v>
-      </c>
-      <c r="B86" s="0" t="n">
-        <v>8</v>
+        <v>907</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>909</v>
-      </c>
-      <c r="B87" s="0" t="n">
-        <v>1</v>
+        <v>908</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>888</v>
+        <v>856</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B88" s="0" t="n">
-        <v>2</v>
+        <v>909</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E88" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>910</v>
       </c>
-      <c r="B89" s="0" t="n">
-        <v>4</v>
+      <c r="B89" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>888</v>
+        <v>856</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B90" s="0" t="n">
-        <v>6</v>
+        <v>911</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>912</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B91" s="0" t="n">
-        <v>8</v>
+        <v>913</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>888</v>
+        <v>861</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B92" s="0" t="n">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>912</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B93" s="0" t="n">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>914</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>910</v>
-      </c>
-      <c r="B94" s="0" t="n">
-        <v>14</v>
+        <v>66</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>864</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B95" s="0" t="n">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>100</v>
+        <v>874</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>184</v>
       </c>
       <c r="E95" s="3" t="n">
-        <f aca="false">D95/B95</f>
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B96" s="0" t="n">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>428</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D96" s="3" t="n">
-        <v>300</v>
+        <v>874</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>293</v>
       </c>
       <c r="E96" s="3" t="n">
-        <f aca="false">D96/B96</f>
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B97" s="0" t="n">
-        <v>3</v>
+        <v>66</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D97" s="3" t="n">
-        <v>600</v>
+        <v>874</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>293</v>
       </c>
       <c r="E97" s="3" t="n">
-        <f aca="false">D97/B97</f>
-        <v>200</v>
+        <v>0</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B98" s="0" t="n">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D98" s="3" t="n">
-        <v>800</v>
+        <v>874</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>133</v>
       </c>
       <c r="E98" s="3" t="n">
-        <f aca="false">D98/B98</f>
-        <v>200</v>
+        <v>0</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B99" s="0" t="n">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D99" s="3" t="n">
-        <v>1000</v>
+        <v>874</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>133</v>
       </c>
       <c r="E99" s="3" t="n">
-        <f aca="false">D99/B99</f>
-        <v>200</v>
+        <v>0</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B100" s="0" t="n">
-        <v>6</v>
+        <v>66</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D100" s="3" t="n">
-        <v>1500</v>
+        <v>874</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="E100" s="3" t="n">
-        <f aca="false">D100/B100</f>
-        <v>250</v>
+        <v>0</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B101" s="0" t="n">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D101" s="3" t="n">
-        <v>2000</v>
+        <v>874</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="E101" s="3" t="n">
-        <f aca="false">D101/B101</f>
-        <v>285.714285714286</v>
+        <v>0</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B102" s="0" t="n">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D102" s="3" t="n">
-        <v>2500</v>
+        <v>874</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="E102" s="3" t="n">
-        <f aca="false">D102/B102</f>
-        <v>312.5</v>
+        <v>0</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B103" s="0" t="n">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D103" s="3" t="n">
-        <v>3000</v>
+        <v>874</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>915</v>
       </c>
       <c r="E103" s="3" t="n">
-        <f aca="false">D103/B103</f>
-        <v>333.333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B104" s="0" t="n">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D104" s="3" t="n">
-        <v>3500</v>
+        <v>874</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>274</v>
       </c>
       <c r="E104" s="3" t="n">
-        <f aca="false">D104/B104</f>
-        <v>350</v>
+        <v>0</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>911</v>
-      </c>
-      <c r="B105" s="0" t="n">
-        <v>11</v>
+        <v>916</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D105" s="3" t="n">
-        <v>4000</v>
+        <v>856</v>
       </c>
       <c r="E105" s="3" t="n">
-        <f aca="false">D105/B105</f>
-        <v>363.636363636364</v>
+        <v>0</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B106" s="0" t="n">
-        <v>1</v>
+        <v>916</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D106" s="3" t="n">
-        <v>1000</v>
+        <v>856</v>
       </c>
       <c r="E106" s="3" t="n">
-        <f aca="false">D106/B106</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B107" s="0" t="n">
-        <v>2</v>
+        <v>916</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D107" s="3" t="n">
-        <v>2000</v>
+        <v>856</v>
       </c>
       <c r="E107" s="3" t="n">
-        <f aca="false">D107/B107</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B108" s="0" t="n">
-        <v>3</v>
+        <v>917</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D108" s="3" t="n">
-        <v>3000</v>
+        <v>856</v>
       </c>
       <c r="E108" s="3" t="n">
-        <f aca="false">D108/B108</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B109" s="0" t="n">
-        <v>4</v>
+        <v>917</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D109" s="3" t="n">
-        <v>4000</v>
+        <v>856</v>
       </c>
       <c r="E109" s="3" t="n">
-        <f aca="false">D109/B109</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B110" s="0" t="n">
-        <v>5</v>
+        <v>917</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D110" s="3" t="n">
-        <v>5000</v>
+        <v>856</v>
       </c>
       <c r="E110" s="3" t="n">
-        <f aca="false">D110/B110</f>
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="B111" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="B111" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="C111" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D111" s="3" t="n">
-        <v>7500</v>
+        <v>874</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>919</v>
       </c>
       <c r="E111" s="3" t="n">
-        <f aca="false">D111/B111</f>
-        <v>1250</v>
+        <v>0</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B112" s="0" t="n">
-        <v>7</v>
+        <v>918</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>864</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D112" s="3" t="n">
-        <v>10000</v>
+        <v>874</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>920</v>
       </c>
       <c r="E112" s="3" t="n">
-        <f aca="false">D112/B112</f>
-        <v>1428.57142857143</v>
+        <v>0</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B113" s="0" t="n">
-        <v>8</v>
+        <v>918</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>428</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D113" s="3" t="n">
-        <v>12500</v>
+        <v>874</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>921</v>
       </c>
       <c r="E113" s="3" t="n">
-        <f aca="false">D113/B113</f>
-        <v>1562.5</v>
+        <v>0</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B114" s="0" t="n">
-        <v>9</v>
+        <v>918</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D114" s="3" t="n">
-        <v>15000</v>
+        <v>874</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>922</v>
       </c>
       <c r="E114" s="3" t="n">
-        <f aca="false">D114/B114</f>
-        <v>1666.66666666667</v>
+        <v>0</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B115" s="0" t="n">
-        <v>10</v>
+        <v>918</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D115" s="3" t="n">
-        <v>17500</v>
+        <v>874</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>923</v>
       </c>
       <c r="E115" s="3" t="n">
-        <f aca="false">D115/B115</f>
-        <v>1750</v>
+        <v>0</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B116" s="0" t="n">
-        <v>11</v>
+        <v>918</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>888</v>
-      </c>
-      <c r="D116" s="3" t="n">
-        <v>20000</v>
+        <v>874</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>924</v>
       </c>
       <c r="E116" s="3" t="n">
-        <f aca="false">D116/B116</f>
-        <v>1818.18181818182</v>
+        <v>0</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B117" s="0" t="n">
-        <v>2</v>
+        <v>925</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>888</v>
+        <v>856</v>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B118" s="0" t="n">
-        <v>3</v>
+        <v>926</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>580</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B119" s="0" t="n">
-        <v>4</v>
+        <v>926</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>539</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B120" s="0" t="n">
-        <v>5</v>
+        <v>926</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>858</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B121" s="0" t="n">
-        <v>6</v>
+        <v>926</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>859</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>888</v>
+        <v>874</v>
+      </c>
+      <c r="E121" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>913</v>
-      </c>
-      <c r="B122" s="0" t="n">
-        <v>7</v>
+        <v>927</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>928</v>
+      </c>
+      <c r="E122" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>914</v>
-      </c>
-      <c r="B123" s="0" t="n">
-        <v>3</v>
+        <v>927</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>861</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="E123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>916</v>
-      </c>
-      <c r="B124" s="0" t="n">
-        <v>3</v>
+        <v>927</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>915</v>
+        <v>861</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="E124" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>917</v>
-      </c>
-      <c r="B125" s="0" t="n">
-        <v>5</v>
+        <v>927</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>915</v>
+        <v>861</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="E125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>918</v>
-      </c>
-      <c r="B126" s="0" t="n">
-        <v>7</v>
+        <v>927</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>915</v>
+        <v>861</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="E126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>919</v>
-      </c>
-      <c r="B127" s="0" t="n">
-        <v>9</v>
+        <v>933</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>920</v>
-      </c>
-      <c r="B128" s="0" t="n">
-        <v>11</v>
+        <v>933</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>428</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>921</v>
-      </c>
-      <c r="B129" s="0" t="n">
-        <v>13</v>
+        <v>933</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>922</v>
-      </c>
-      <c r="B130" s="0" t="n">
-        <v>3</v>
+        <v>933</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>923</v>
-      </c>
-      <c r="B131" s="0" t="n">
-        <v>5</v>
+        <v>933</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="B132" s="0" t="n">
-        <v>7</v>
+        <v>933</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>925</v>
-      </c>
-      <c r="B133" s="0" t="n">
-        <v>9</v>
+        <v>933</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>926</v>
-      </c>
-      <c r="B134" s="0" t="n">
-        <v>11</v>
+        <v>933</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>927</v>
-      </c>
-      <c r="B135" s="0" t="n">
-        <v>13</v>
+        <v>933</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>928</v>
-      </c>
-      <c r="B136" s="0" t="n">
-        <v>3</v>
+        <v>933</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>915</v>
+        <v>874</v>
+      </c>
+      <c r="E136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>929</v>
-      </c>
-      <c r="B137" s="0" t="n">
-        <v>5</v>
+        <v>934</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>915</v>
+        <v>670</v>
+      </c>
+      <c r="E137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>930</v>
-      </c>
-      <c r="B138" s="0" t="n">
-        <v>7</v>
+        <v>935</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>915</v>
+        <v>861</v>
+      </c>
+      <c r="E138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>931</v>
-      </c>
-      <c r="B139" s="0" t="n">
-        <v>9</v>
+        <v>936</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>429</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>861</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>937</v>
+      </c>
+      <c r="E139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="E140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="E141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D142" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="E142" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="E143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E146" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>943</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E148" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E150" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E152" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E153" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E154" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E157" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C159" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E159" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="C160" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="C161" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="E161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>947</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C162" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E162" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>948</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="C163" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E163" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>949</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C164" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E164" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="E165" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>951</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>952</v>
+      </c>
+      <c r="E166" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>951</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>953</v>
+      </c>
+      <c r="E167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E168" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E169" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E170" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E171" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E173" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E174" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="E175" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>857</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>